<commit_message>
Qui se charge de quelle classe
</commit_message>
<xml_diff>
--- a/To Do list.xlsx
+++ b/To Do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B59FF81-E2C5-4373-BF80-3EB5B5F373CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72638990-7F24-4344-BA37-49FDD795231B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Tâche</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Camille</t>
-  </si>
-  <si>
-    <t>À re vérifier</t>
   </si>
   <si>
     <t>Faire Use case</t>
@@ -76,25 +73,13 @@
     <t>Ajouter les IA</t>
   </si>
   <si>
-    <t>identifier commentaires positifs ou négatif</t>
-  </si>
-  <si>
-    <t>faire moyenne des score dans Movie</t>
-  </si>
-  <si>
     <t>des calculs de stats de Bdd</t>
-  </si>
-  <si>
-    <t>trier par ordre chronologique commentaires dans Movie</t>
   </si>
   <si>
     <t>Ajouter class panier</t>
   </si>
   <si>
     <t>Ajouter attributs à Movie</t>
-  </si>
-  <si>
-    <t>attribut prix en long</t>
   </si>
   <si>
     <t>Ajouter attributs à User</t>
@@ -108,6 +93,30 @@
   <si>
     <t>dans l'UML et dans le code</t>
   </si>
+  <si>
+    <t>Franklin</t>
+  </si>
+  <si>
+    <t>classes User et Admin</t>
+  </si>
+  <si>
+    <t>classes Bdd, Factures et Panier</t>
+  </si>
+  <si>
+    <t>trier par ordre chronologique les commentaires dans Movie</t>
+  </si>
+  <si>
+    <t>attribut prix, type --&gt; long</t>
+  </si>
+  <si>
+    <t>identifier commentaires positifs ou négatifs</t>
+  </si>
+  <si>
+    <t>faire moyenne des scores dans Movie</t>
+  </si>
+  <si>
+    <t>class Score, Comment, Movie et Person</t>
+  </si>
 </sst>
 </file>
 
@@ -116,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -134,6 +143,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -163,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -191,6 +214,12 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,9 +515,9 @@
   </sheetPr>
   <dimension ref="A1:Y970"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="146" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -499,7 +528,7 @@
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,56 +565,19 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="5">
-        <v>45383</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-    </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="5">
         <v>45383</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -610,15 +602,17 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -642,14 +636,18 @@
       <c r="Y4" s="3"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>15</v>
+      <c r="A5" s="8" t="s">
+        <v>11</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -672,15 +670,19 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
+    <row r="6" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>11</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -704,14 +706,18 @@
       <c r="Y6" s="3"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
+      <c r="A7" s="10" t="s">
+        <v>19</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -735,16 +741,18 @@
       <c r="Y7" s="3"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>12</v>
+      <c r="A8" s="10" t="s">
+        <v>11</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
+      <c r="B8" s="10" t="s">
+        <v>29</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -768,16 +776,18 @@
       <c r="Y8" s="3"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>12</v>
+      <c r="A9" s="10" t="s">
+        <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
+      <c r="B9" s="10" t="s">
+        <v>30</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -801,16 +811,18 @@
       <c r="Y9" s="3"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>12</v>
+      <c r="A10" s="10" t="s">
+        <v>11</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
+      <c r="B10" s="10" t="s">
+        <v>31</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -833,17 +845,19 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
     </row>
-    <row r="11" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>12</v>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>21</v>
+      <c r="B11" s="11" t="s">
+        <v>6</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -868,13 +882,15 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -899,15 +915,15 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
       </c>
-      <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -931,16 +947,18 @@
       <c r="Y13" s="3"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>25</v>
+      <c r="A14" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -965,15 +983,15 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>28</v>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>7</v>
       </c>
-      <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -997,11 +1015,19 @@
       <c r="Y15" s="3"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1024,11 +1050,19 @@
       <c r="Y16" s="3"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1051,11 +1085,17 @@
       <c r="Y17" s="3"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1078,11 +1118,15 @@
       <c r="Y18" s="3"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1103,303 +1147,6 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-      <c r="V27" s="3"/>
-      <c r="W27" s="3"/>
-      <c r="X27" s="3"/>
-      <c r="Y27" s="3"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="W28" s="3"/>
-      <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
-      <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
@@ -26782,49 +26529,50 @@
       <c r="Y970" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:B970">
+  <conditionalFormatting sqref="A31:B970 A3:B19">
     <cfRule type="expression" dxfId="6" priority="1">
-      <formula>$E2="Terminé"</formula>
+      <formula>$E3="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D970">
+  <conditionalFormatting sqref="D31:D970 D3:D19">
     <cfRule type="expression" dxfId="5" priority="2">
-      <formula>AND(TODAY()=$D2,NOT($D2=""),$E2&lt;&gt;"Terminé")</formula>
+      <formula>AND(TODAY()=$D3,NOT($D3=""),$E3&lt;&gt;"Terminé")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D970">
+  <conditionalFormatting sqref="D31:D970 D3:D19">
     <cfRule type="expression" dxfId="4" priority="3">
-      <formula>AND(NOW()&gt;$D2,NOT($D2=""),$E2&lt;&gt;"Terminé",$E2&lt;&gt;"À re vérifier")</formula>
+      <formula>AND(NOW()&gt;$D3,NOT($D3=""),$E3&lt;&gt;"Terminé",$E3&lt;&gt;"À re vérifier")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:B970">
+  <conditionalFormatting sqref="A31:B970 A3:B19">
     <cfRule type="expression" dxfId="3" priority="4">
-      <formula>$E2="À re vérifier"</formula>
+      <formula>$E3="À re vérifier"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:B970">
+  <conditionalFormatting sqref="A31:B970 A3:B19">
     <cfRule type="expression" dxfId="2" priority="5">
-      <formula>$C2="Camille"</formula>
+      <formula>$C3="Camille"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:B970">
+  <conditionalFormatting sqref="A31:B970 A3:B19">
     <cfRule type="expression" dxfId="1" priority="6">
-      <formula>$C2="Edner"</formula>
+      <formula>$C3="Edner"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:B970">
+  <conditionalFormatting sqref="A31:B970 A3:B19">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula>$C2="Franklin"</formula>
+      <formula>$C3="Franklin"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C970" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C31:C970 C3:C19" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Camille,Edner,Franklin"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E970" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E31:E970 E3:E19" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"En attente,Attribué,En cours,À re vérifier,Terminé"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>